<commit_message>
adding blank run 17
</commit_message>
<xml_diff>
--- a/QPCR_Plate_Logs.xlsx
+++ b/QPCR_Plate_Logs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13120" windowHeight="13620" tabRatio="500" firstSheet="12" activeTab="15"/>
+    <workbookView xWindow="7700" yWindow="0" windowWidth="13120" windowHeight="13620" tabRatio="500" firstSheet="16" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="03-13-18-Run3" sheetId="6" r:id="rId1"/>
@@ -23,10 +23,11 @@
     <sheet name="2018-03-17-Run14" sheetId="19" r:id="rId14"/>
     <sheet name="2018-03-17-Run15" sheetId="20" r:id="rId15"/>
     <sheet name="2018-09-20-Run16" sheetId="21" r:id="rId16"/>
-    <sheet name="Master Mix Calculation" sheetId="3" r:id="rId17"/>
+    <sheet name="2018-09-27-Run17" sheetId="22" r:id="rId17"/>
+    <sheet name="Master Mix Calculation" sheetId="3" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'Master Mix Calculation'!$A$1:$G$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'Master Mix Calculation'!$A$1:$G$7</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'03-02-18-Run4'!$A$1:$N$21</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'03-13-18-Run7'!$A$1:$M$23</definedName>
   </definedNames>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="717">
   <si>
     <t>target</t>
   </si>
@@ -8255,8 +8256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8964,6 +8965,550 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="6.83203125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" style="39" customWidth="1"/>
+    <col min="13" max="13" width="6.83203125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="8.5" style="4" customWidth="1"/>
+    <col min="15" max="15" width="8.6640625" style="4"/>
+    <col min="16" max="16" width="19.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" style="4"/>
+    <col min="19" max="19" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" style="4"/>
+    <col min="21" max="21" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.6640625" style="4"/>
+    <col min="23" max="23" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.6640625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" ht="15">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="8"/>
+    </row>
+    <row r="2" spans="1:32" ht="31.5" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="12"/>
+      <c r="P2"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="13"/>
+      <c r="Z2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="14">
+        <v>213000000</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="14">
+        <v>213000</v>
+      </c>
+      <c r="AD2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="14">
+        <v>213</v>
+      </c>
+      <c r="AF2" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="31.5" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="16"/>
+      <c r="P3"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="17"/>
+    </row>
+    <row r="4" spans="1:32" ht="31.5" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="16"/>
+      <c r="P4"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="22"/>
+    </row>
+    <row r="5" spans="1:32" ht="31.5" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="23"/>
+      <c r="P5"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="17"/>
+    </row>
+    <row r="6" spans="1:32" ht="31.5" customHeight="1">
+      <c r="A6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="16"/>
+      <c r="P6"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="17"/>
+    </row>
+    <row r="7" spans="1:32" ht="31.5" customHeight="1">
+      <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="16"/>
+      <c r="P7"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="22"/>
+    </row>
+    <row r="8" spans="1:32" ht="31.5" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="16"/>
+      <c r="P8"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="17"/>
+    </row>
+    <row r="9" spans="1:32" ht="31.5" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="16"/>
+      <c r="P9"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="17"/>
+    </row>
+    <row r="10" spans="1:32" ht="31.5" customHeight="1">
+      <c r="A10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10"/>
+    </row>
+    <row r="11" spans="1:32" ht="16" thickBot="1">
+      <c r="L11" s="35"/>
+      <c r="P11"/>
+    </row>
+    <row r="12" spans="1:32" ht="15">
+      <c r="B12" s="40"/>
+      <c r="C12" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41">
+        <v>101</v>
+      </c>
+      <c r="L12" s="36"/>
+      <c r="N12" s="35"/>
+      <c r="P12"/>
+    </row>
+    <row r="13" spans="1:32">
+      <c r="B13" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43">
+        <v>2.5</v>
+      </c>
+      <c r="G13" s="44"/>
+      <c r="H13" s="45">
+        <f>F13*H12</f>
+        <v>252.5</v>
+      </c>
+      <c r="L13" s="35"/>
+      <c r="N13" s="37"/>
+    </row>
+    <row r="14" spans="1:32" ht="55">
+      <c r="B14" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43">
+        <v>5</v>
+      </c>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45">
+        <f>F14*H12</f>
+        <v>505</v>
+      </c>
+      <c r="L14" s="36"/>
+    </row>
+    <row r="15" spans="1:32">
+      <c r="B15" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="46"/>
+      <c r="F15" s="43">
+        <v>0.25</v>
+      </c>
+      <c r="G15" s="44"/>
+      <c r="H15" s="45">
+        <f>F15*H12</f>
+        <v>25.25</v>
+      </c>
+      <c r="L15" s="35"/>
+    </row>
+    <row r="16" spans="1:32">
+      <c r="B16" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="46"/>
+      <c r="F16" s="43">
+        <v>0.25</v>
+      </c>
+      <c r="G16" s="44"/>
+      <c r="H16" s="45">
+        <f>F16*H12</f>
+        <v>25.25</v>
+      </c>
+      <c r="L16" s="35"/>
+    </row>
+    <row r="17" spans="2:12" ht="31.5" customHeight="1">
+      <c r="B17" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43">
+        <v>2</v>
+      </c>
+      <c r="G17" s="47"/>
+      <c r="H17" s="45">
+        <f>F17</f>
+        <v>2</v>
+      </c>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="2:12" ht="31.5" customHeight="1" thickBot="1">
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="2:12" ht="31.5" customHeight="1">
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="B20" s="52" t="s">
+        <v>673</v>
+      </c>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="B21" s="53" t="s">
+        <v>674</v>
+      </c>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="2:12">
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="2:12">
+      <c r="L29" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>

</xml_diff>

<commit_message>
Addition of 8-17 --> 10-17
Dilution template done, still need to do the CRX, and qPCR Log plates
</commit_message>
<xml_diff>
--- a/QPCR_Plate_Logs.xlsx
+++ b/QPCR_Plate_Logs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymond/Desktop/Frawgz/qPCR_Lab_Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E3F189-FB1C-4042-AC25-5B805CBC91E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0619F99C-8BD8-8644-A41B-E4941122C273}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14960" windowHeight="13620" tabRatio="500" firstSheet="29" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18480" windowHeight="14440" tabRatio="500" firstSheet="29" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2018-03-14-Run1" sheetId="2" r:id="rId1"/>
@@ -45,15 +45,21 @@
     <sheet name="2018-11-21-Run5-17" sheetId="37" r:id="rId30"/>
     <sheet name="2018-11-21-Run6-17" sheetId="38" r:id="rId31"/>
     <sheet name="2018-12-6-Run7-17" sheetId="39" r:id="rId32"/>
-    <sheet name="Master Mix Calculation" sheetId="3" r:id="rId33"/>
+    <sheet name="2018-12-6-Run8-17" sheetId="41" r:id="rId33"/>
+    <sheet name="Master Mix Calculation" sheetId="3" r:id="rId34"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="32" hidden="1">'Master Mix Calculation'!$A$1:$G$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">'Master Mix Calculation'!$A$1:$G$7</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'03-02-18-Run4'!$A$1:$N$21</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'03-13-18-Run7'!$A$1:$M$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -62,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4076" uniqueCount="1389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4203" uniqueCount="1430">
   <si>
     <t>target</t>
   </si>
@@ -4290,6 +4296,129 @@
   </si>
   <si>
     <t>L2-1-8</t>
+  </si>
+  <si>
+    <t>X2-1-14</t>
+  </si>
+  <si>
+    <t>I2-1-17</t>
+  </si>
+  <si>
+    <t>K2-1-11</t>
+  </si>
+  <si>
+    <t>A2-1-12</t>
+  </si>
+  <si>
+    <t>CC2-1-11</t>
+  </si>
+  <si>
+    <t>T2-1-15</t>
+  </si>
+  <si>
+    <t>F2-1-19</t>
+  </si>
+  <si>
+    <t>C2-1-7</t>
+  </si>
+  <si>
+    <t>CC2-1-22</t>
+  </si>
+  <si>
+    <t>U2-1-16</t>
+  </si>
+  <si>
+    <t>AA2-1-18</t>
+  </si>
+  <si>
+    <t>P2-1-3</t>
+  </si>
+  <si>
+    <t>C2-1-17</t>
+  </si>
+  <si>
+    <t>CC2-1-24</t>
+  </si>
+  <si>
+    <t>J2-1-6</t>
+  </si>
+  <si>
+    <t>Q2-1-21</t>
+  </si>
+  <si>
+    <t>T2-1-2</t>
+  </si>
+  <si>
+    <t>C2-1-5</t>
+  </si>
+  <si>
+    <t>X2-1-28</t>
+  </si>
+  <si>
+    <t>I2-1-3</t>
+  </si>
+  <si>
+    <t>K2-1-9</t>
+  </si>
+  <si>
+    <t>S2-1-15</t>
+  </si>
+  <si>
+    <t>S2-1-11</t>
+  </si>
+  <si>
+    <t>V2-1-22</t>
+  </si>
+  <si>
+    <t>W2-1-9</t>
+  </si>
+  <si>
+    <t>CC2-1-30</t>
+  </si>
+  <si>
+    <t>Q2-1-11</t>
+  </si>
+  <si>
+    <t>E2-1-19</t>
+  </si>
+  <si>
+    <t>Y2-1-26</t>
+  </si>
+  <si>
+    <t>G2-1-7</t>
+  </si>
+  <si>
+    <t>G2-1-3</t>
+  </si>
+  <si>
+    <t>U2-1-12</t>
+  </si>
+  <si>
+    <t>N2-1-28</t>
+  </si>
+  <si>
+    <t>V2-1-3</t>
+  </si>
+  <si>
+    <t>X2-1-29</t>
+  </si>
+  <si>
+    <t>U2-1-22</t>
+  </si>
+  <si>
+    <t>G2-1-6</t>
+  </si>
+  <si>
+    <t>I2-1-29</t>
+  </si>
+  <si>
+    <t>U2-1-13</t>
+  </si>
+  <si>
+    <t>I2-1-22</t>
+  </si>
+  <si>
+    <t>E2-1-20</t>
   </si>
 </sst>
 </file>
@@ -23049,8 +23178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D29717B-CF1F-1B41-99E3-4A881132991F}">
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23753,6 +23882,713 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A507C1-2800-574F-8766-9BC933C3BBDD}">
+  <dimension ref="A1:AF29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="7.1640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" style="39" customWidth="1"/>
+    <col min="13" max="13" width="7.1640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="8.5" style="4" customWidth="1"/>
+    <col min="15" max="15" width="8.6640625" style="4"/>
+    <col min="16" max="16" width="19.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" style="4"/>
+    <col min="19" max="19" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" style="4"/>
+    <col min="21" max="21" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.6640625" style="4"/>
+    <col min="23" max="23" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.6640625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="8"/>
+    </row>
+    <row r="2" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>1389</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>1390</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>1391</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>1392</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>1393</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="12"/>
+      <c r="P2"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="13"/>
+      <c r="Z2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="14">
+        <v>213000000</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="14">
+        <v>213000</v>
+      </c>
+      <c r="AD2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="14">
+        <v>213</v>
+      </c>
+      <c r="AF2" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>1389</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>1390</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>1391</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>1392</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>1393</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>1394</v>
+      </c>
+      <c r="N3" s="18"/>
+      <c r="O3" s="16"/>
+      <c r="P3"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="17"/>
+    </row>
+    <row r="4" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>1400</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>1401</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>1402</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>1403</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>1404</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>1405</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>1406</v>
+      </c>
+      <c r="N4" s="18"/>
+      <c r="O4" s="16"/>
+      <c r="P4"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="22"/>
+    </row>
+    <row r="5" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>1400</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>1401</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>1402</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>1403</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>1404</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>1405</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>1406</v>
+      </c>
+      <c r="N5" s="23"/>
+      <c r="P5"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="17"/>
+    </row>
+    <row r="6" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>1409</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>1412</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>1413</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>1414</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>1415</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>1416</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>1417</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>1418</v>
+      </c>
+      <c r="N6" s="18"/>
+      <c r="O6" s="16"/>
+      <c r="P6"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="17"/>
+    </row>
+    <row r="7" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>1409</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>1412</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>1413</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>1414</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>1415</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>1416</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>1417</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>1418</v>
+      </c>
+      <c r="N7" s="18"/>
+      <c r="O7" s="16"/>
+      <c r="P7"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="22"/>
+    </row>
+    <row r="8" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>1421</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>1422</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>1423</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>1424</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>1425</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>1426</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>1427</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>1155</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>1428</v>
+      </c>
+      <c r="M8" s="26" t="s">
+        <v>1429</v>
+      </c>
+      <c r="N8" s="23"/>
+      <c r="O8" s="16"/>
+      <c r="P8"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="17"/>
+    </row>
+    <row r="9" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>1421</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>1422</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>1423</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>1424</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>1425</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>1426</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>1427</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>1155</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>1428</v>
+      </c>
+      <c r="M9" s="26" t="s">
+        <v>1429</v>
+      </c>
+      <c r="N9" s="29"/>
+      <c r="O9" s="16"/>
+      <c r="P9"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="17"/>
+    </row>
+    <row r="10" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10"/>
+    </row>
+    <row r="11" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L11" s="35"/>
+      <c r="P11"/>
+    </row>
+    <row r="12" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+      <c r="B12" s="40"/>
+      <c r="C12" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41">
+        <v>101</v>
+      </c>
+      <c r="L12" s="36"/>
+      <c r="N12" s="35"/>
+      <c r="P12"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="B13" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43">
+        <v>2.5</v>
+      </c>
+      <c r="G13" s="44"/>
+      <c r="H13" s="45">
+        <f>F13*H12</f>
+        <v>252.5</v>
+      </c>
+      <c r="L13" s="35"/>
+      <c r="N13" s="37"/>
+    </row>
+    <row r="14" spans="1:32" ht="60" x14ac:dyDescent="0.2">
+      <c r="B14" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43">
+        <v>5</v>
+      </c>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45">
+        <f>F14*H12</f>
+        <v>505</v>
+      </c>
+      <c r="L14" s="36"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="B15" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="46"/>
+      <c r="F15" s="43">
+        <v>0.25</v>
+      </c>
+      <c r="G15" s="44"/>
+      <c r="H15" s="45">
+        <f>F15*H12</f>
+        <v>25.25</v>
+      </c>
+      <c r="L15" s="35"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="B16" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="46"/>
+      <c r="F16" s="43">
+        <v>0.25</v>
+      </c>
+      <c r="G16" s="44"/>
+      <c r="H16" s="45">
+        <f>F16*H12</f>
+        <v>25.25</v>
+      </c>
+      <c r="L16" s="35"/>
+    </row>
+    <row r="17" spans="2:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43">
+        <v>2</v>
+      </c>
+      <c r="G17" s="47"/>
+      <c r="H17" s="45">
+        <f>F17</f>
+        <v>2</v>
+      </c>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="2:12" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="2:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B20" s="52" t="s">
+        <v>673</v>
+      </c>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21" s="53" t="s">
+        <v>674</v>
+      </c>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L29" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>

</xml_diff>